<commit_message>
Merge the cell description function by Prerna.
</commit_message>
<xml_diff>
--- a/sample_excel_files/hidden_cells_key_1.xlsx
+++ b/sample_excel_files/hidden_cells_key_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93E3DE-4F1D-A54C-B870-FB335D6F3AEB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C002548-DF5F-2F43-8FDA-07D7FC550148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1260" yWindow="4940" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="3" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Answer</t>
   </si>
@@ -247,9 +247,6 @@
   </si>
   <si>
     <t>check student's answer for zipcode of Columbus</t>
-  </si>
-  <si>
-    <t>check student's answer for zipcode of New York</t>
   </si>
   <si>
     <t>check student's answer for zipcode of Mountain View</t>
@@ -716,7 +713,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,10 +730,10 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -750,7 +747,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -760,11 +757,8 @@
       <c r="B3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -775,7 +769,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Display hidden cell's hint if the cell is not passed
</commit_message>
<xml_diff>
--- a/sample_excel_files/hidden_cells_key_1.xlsx
+++ b/sample_excel_files/hidden_cells_key_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfa/workspace/pysheetgrader/sample_excel_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C002548-DF5F-2F43-8FDA-07D7FC550148}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893CA102-D297-284C-836F-865F297069F6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1260" yWindow="4940" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-35500" yWindow="1040" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SheetGradingOrder" sheetId="3" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Answer</t>
   </si>
@@ -262,6 +262,18 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>Feedback (Optional)</t>
+  </si>
+  <si>
+    <t>This hidden cell has failed for checking Columbus zipcode</t>
+  </si>
+  <si>
+    <t>This hidden cell has failed for checking Mountain View zipcode</t>
+  </si>
+  <si>
+    <t>This hidden cell has failed for checking New York zipcode</t>
   </si>
 </sst>
 </file>
@@ -710,19 +722,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="45" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" customWidth="1"/>
+    <col min="5" max="5" width="55.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -735,8 +748,11 @@
       <c r="D1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -749,8 +765,11 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -760,8 +779,11 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -770,6 +792,9 @@
       </c>
       <c r="C4" t="s">
         <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>